<commit_message>
Changesd done on 25th March
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smit.rathore\Documents\UiPath\WI4-Performer-Canberra-Deloitte\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1859C9C-4607-4481-A324-EFC39DB1E89D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD7D2F6-396E-438B-BE64-C0FA05BDA01F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8085" yWindow="2865" windowWidth="19200" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="1260" windowWidth="19200" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>ACME_CREDENTIALS</t>
+  </si>
+  <si>
+    <t>DownloadFilePath</t>
+  </si>
+  <si>
+    <t>Data\Temp</t>
   </si>
 </sst>
 </file>
@@ -515,7 +521,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -613,7 +619,14 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -1608,7 +1621,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2719,7 +2734,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>